<commit_message>
Adding segment3 files for dashboard and ppt
</commit_message>
<xml_diff>
--- a/Segment2/ML_Models_Chronological - Tableau.xlsx
+++ b/Segment2/ML_Models_Chronological - Tableau.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuti\Desktop\Class Folder\MODULE20_FinalProject\UCB_COVID_Prediction_Model\UCB_COVID_Prediction_Model\Segment2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuti\Desktop\Class Folder\MODULE20_FinalProject_NEQ\UCB_COVID_Prediction_Model\Segment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA75E427-D6E8-4A0C-9FE2-5327C702DA97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009505A4-DF2B-41E4-8C01-D246DA573EBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23370" yWindow="1065" windowWidth="20460" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance@30-50Epochs" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Loss</t>
   </si>
@@ -148,6 +148,15 @@
   <si>
     <t>Model. 
 No.</t>
+  </si>
+  <si>
+    <t>Model 10</t>
+  </si>
+  <si>
+    <t>Resnet-C</t>
+  </si>
+  <si>
+    <t>Model10_history</t>
   </si>
 </sst>
 </file>
@@ -233,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,6 +270,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -546,7 +558,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,8 +865,33 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0.3841</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.84719999999999995</v>
+      </c>
+      <c r="G11" s="12">
+        <v>0.4577</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.83040000000000003</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -927,7 +964,9 @@
     <hyperlink ref="I8" r:id="rId7" xr:uid="{7FB6EAAD-CEAF-480C-BF93-728226BFE0F8}"/>
     <hyperlink ref="I10" r:id="rId8" xr:uid="{788C7286-1EFA-4EEE-BA8F-380B814A0EB9}"/>
     <hyperlink ref="I7" r:id="rId9" xr:uid="{5F48B62D-84DA-47A1-A5BE-2E8834ED8856}"/>
+    <hyperlink ref="I11" r:id="rId10" xr:uid="{338977F2-3845-4E51-B7AF-CD97468AEC52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>